<commit_message>
Más analisis de datos
</commit_message>
<xml_diff>
--- a/Experimento a presentar/SternGerlach/TablasDatos.xlsx
+++ b/Experimento a presentar/SternGerlach/TablasDatos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feyra\Desktop\UNI\T-cnicas-experimentales-II\Experimento a presentar\SternGerlach\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Carpetas de datos\Desktop\UNI-Alicante\T-cnicas-experimentales-II\Experimento a presentar\SternGerlach\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44C0149-BAC3-444C-BE6F-6F8440F0F233}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4817A558-81F1-4207-9CE7-741C9CE18F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prueba preliminar" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -7775,16 +7784,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1200149</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>32385</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>617220</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7812,13 +7821,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>396240</xdr:colOff>
+      <xdr:colOff>320040</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
+      <xdr:colOff>137160</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
@@ -8149,16 +8158,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="41.6640625" customWidth="1"/>
+    <col min="5" max="5" width="41.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -8178,7 +8187,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>80</v>
       </c>
@@ -8186,7 +8195,7 @@
         <v>7.44</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>65</v>
       </c>
@@ -8203,7 +8212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>50</v>
       </c>
@@ -8211,7 +8220,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>35</v>
       </c>
@@ -8219,7 +8228,7 @@
         <v>4.58</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>20</v>
       </c>
@@ -8227,7 +8236,7 @@
         <v>3.15</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>5</v>
       </c>
@@ -8235,7 +8244,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>-10</v>
       </c>
@@ -8243,7 +8252,7 @@
         <v>1.71</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>-25</v>
       </c>
@@ -8251,7 +8260,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>-40</v>
       </c>
@@ -8259,7 +8268,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>-55</v>
       </c>
@@ -8267,7 +8276,7 @@
         <v>4.57</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>-70</v>
       </c>
@@ -8275,7 +8284,7 @@
         <v>6.01</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>-80</v>
       </c>
@@ -8283,7 +8292,7 @@
         <v>6.76</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>1</v>
       </c>
@@ -8300,62 +8309,62 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>-10</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>-25</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>-40</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>-55</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>-70</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>-80</v>
       </c>
@@ -8374,14 +8383,14 @@
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -8419,7 +8428,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -8462,7 +8471,7 @@
         <v>2.5052192066805683E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B4">
         <f>B3+5</f>
         <v>-85</v>
@@ -8492,7 +8501,7 @@
         <v>3.3402922755740971E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B5">
         <f t="shared" ref="B5:B39" si="2">B4+5</f>
         <v>-80</v>
@@ -8516,7 +8525,7 @@
         <v>6.2630480167014571E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B6">
         <f t="shared" si="2"/>
         <v>-75</v>
@@ -8540,7 +8549,7 @@
         <v>9.6033402922755737E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B7">
         <f t="shared" si="2"/>
         <v>-70</v>
@@ -8570,7 +8579,7 @@
         <v>0.13987473903966577</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B8">
         <f t="shared" si="2"/>
         <v>-65</v>
@@ -8600,7 +8609,7 @@
         <v>0.19624217118997919</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B9">
         <f t="shared" si="2"/>
         <v>-60</v>
@@ -8624,7 +8633,7 @@
         <v>0.25887265135699361</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B10">
         <f t="shared" si="2"/>
         <v>-55</v>
@@ -8648,7 +8657,7 @@
         <v>0.32359081419624214</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B11">
         <f t="shared" si="2"/>
         <v>-50</v>
@@ -8672,7 +8681,7 @@
         <v>0.40292275574112713</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B12">
         <f t="shared" si="2"/>
         <v>-45</v>
@@ -8696,7 +8705,7 @@
         <v>0.47807933194154489</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B13">
         <f t="shared" si="2"/>
         <v>-40</v>
@@ -8720,7 +8729,7 @@
         <v>0.55114822546972853</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B14">
         <f t="shared" si="2"/>
         <v>-35</v>
@@ -8744,7 +8753,7 @@
         <v>0.63883089770354895</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B15">
         <f t="shared" si="2"/>
         <v>-30</v>
@@ -8768,7 +8777,7 @@
         <v>0.71607515657620013</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B16">
         <f t="shared" si="2"/>
         <v>-25</v>
@@ -8792,7 +8801,7 @@
         <v>0.78914405010438415</v>
       </c>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17">
         <f t="shared" si="2"/>
         <v>-20</v>
@@ -8816,7 +8825,7 @@
         <v>0.85386221294363229</v>
       </c>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18">
         <f t="shared" si="2"/>
         <v>-15</v>
@@ -8840,7 +8849,7 @@
         <v>0.91858037578288088</v>
       </c>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19">
         <f t="shared" si="2"/>
         <v>-10</v>
@@ -8864,7 +8873,7 @@
         <v>0.96033402922755717</v>
       </c>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20">
         <f t="shared" si="2"/>
         <v>-5</v>
@@ -8888,7 +8897,7 @@
         <v>0.98747390396659696</v>
       </c>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -8912,7 +8921,7 @@
         <v>0.9979123173277662</v>
       </c>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -8936,7 +8945,7 @@
         <v>0.98956158663883076</v>
       </c>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -8960,7 +8969,7 @@
         <v>0.96242171189979131</v>
       </c>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24">
         <f t="shared" si="2"/>
         <v>15</v>
@@ -8984,7 +8993,7 @@
         <v>0.91231732776617958</v>
       </c>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -9008,7 +9017,7 @@
         <v>0.8496868475991648</v>
       </c>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26">
         <f t="shared" si="2"/>
         <v>25</v>
@@ -9032,7 +9041,7 @@
         <v>0.76826722338204567</v>
       </c>
     </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27">
         <f t="shared" si="2"/>
         <v>30</v>
@@ -9056,7 +9065,7 @@
         <v>0.66388308977035471</v>
       </c>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -9080,7 +9089,7 @@
         <v>0.55114822546972853</v>
       </c>
     </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -9104,7 +9113,7 @@
         <v>0.43006263048016691</v>
       </c>
     </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -9128,7 +9137,7 @@
         <v>0.29436325678496855</v>
       </c>
     </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31">
         <f t="shared" si="2"/>
         <v>50</v>
@@ -9152,7 +9161,7 @@
         <v>0.16910229645093938</v>
       </c>
     </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32">
         <f t="shared" si="2"/>
         <v>55</v>
@@ -9176,7 +9185,7 @@
         <v>3.1315240083507195E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B33">
         <f t="shared" si="2"/>
         <v>60</v>
@@ -9200,7 +9209,7 @@
         <v>-9.1858037578288185E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B34">
         <f t="shared" si="2"/>
         <v>65</v>
@@ -9224,7 +9233,7 @@
         <v>-0.20876826722338204</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35">
         <f t="shared" si="2"/>
@@ -9251,7 +9260,7 @@
         <v>-0.27348643006263057</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B36">
         <f t="shared" si="2"/>
         <v>75</v>
@@ -9271,7 +9280,7 @@
         <v>-0.35281837160751572</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B37">
         <f t="shared" si="2"/>
         <v>80</v>
@@ -9291,7 +9300,7 @@
         <v>-0.44676409185803767</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B38">
         <f t="shared" si="2"/>
         <v>85</v>
@@ -9311,7 +9320,7 @@
         <v>-0.48851774530271413</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B39">
         <f t="shared" si="2"/>
         <v>90</v>
@@ -9341,18 +9350,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{229D5F47-CC9B-4815-AB3D-6E4C5984C9C1}">
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:N39"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="20.21875" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>6</v>
       </c>
@@ -9369,7 +9378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -9407,7 +9416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -9445,7 +9454,7 @@
         <v>3.61</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C4">
         <f>C3-5</f>
         <v>5</v>
@@ -9468,9 +9477,9 @@
         <v>3.53</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C5">
-        <f t="shared" ref="C5:C40" si="0">C4-5</f>
+        <f t="shared" ref="C5:C39" si="0">C4-5</f>
         <v>0</v>
       </c>
       <c r="D5">
@@ -9491,7 +9500,7 @@
         <v>3.43</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C6">
         <f t="shared" si="0"/>
         <v>-5</v>
@@ -9514,7 +9523,7 @@
         <v>3.31</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C7">
         <f t="shared" si="0"/>
         <v>-10</v>
@@ -9537,7 +9546,7 @@
         <v>3.19</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C8">
         <f t="shared" si="0"/>
         <v>-15</v>
@@ -9560,7 +9569,7 @@
         <v>3.06</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C9">
         <f t="shared" si="0"/>
         <v>-20</v>
@@ -9583,7 +9592,7 @@
         <v>2.94</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C10">
         <f t="shared" si="0"/>
         <v>-25</v>
@@ -9606,7 +9615,7 @@
         <v>2.81</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C11">
         <f t="shared" si="0"/>
         <v>-30</v>
@@ -9629,7 +9638,7 @@
         <v>2.69</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C12">
         <f t="shared" si="0"/>
         <v>-35</v>
@@ -9652,7 +9661,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C13">
         <f t="shared" si="0"/>
         <v>-40</v>
@@ -9675,7 +9684,7 @@
         <v>2.4900000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C14">
         <f t="shared" si="0"/>
         <v>-45</v>
@@ -9698,7 +9707,7 @@
         <v>2.41</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C15">
         <f t="shared" si="0"/>
         <v>-50</v>
@@ -9721,7 +9730,7 @@
         <v>2.35</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C16">
         <f t="shared" si="0"/>
         <v>-55</v>
@@ -9744,7 +9753,7 @@
         <v>2.3199999999999998</v>
       </c>
     </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C17">
         <f>C16-5</f>
         <v>-60</v>
@@ -9767,7 +9776,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C18">
         <f t="shared" si="0"/>
         <v>-65</v>
@@ -9790,7 +9799,7 @@
         <v>2.31</v>
       </c>
     </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C19">
         <f t="shared" si="0"/>
         <v>-70</v>
@@ -9813,7 +9822,7 @@
         <v>2.34</v>
       </c>
     </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C20">
         <f>C19-5</f>
         <v>-75</v>
@@ -9836,7 +9845,7 @@
         <v>2.38</v>
       </c>
     </row>
-    <row r="21" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C21">
         <f t="shared" si="0"/>
         <v>-80</v>
@@ -9859,7 +9868,7 @@
         <v>2.46</v>
       </c>
     </row>
-    <row r="22" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C22">
         <f t="shared" si="0"/>
         <v>-85</v>
@@ -9882,7 +9891,7 @@
         <v>2.5499999999999998</v>
       </c>
     </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C23">
         <f t="shared" si="0"/>
         <v>-90</v>
@@ -9905,7 +9914,7 @@
         <v>2.66</v>
       </c>
     </row>
-    <row r="24" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C24">
         <f t="shared" si="0"/>
         <v>-95</v>
@@ -9928,7 +9937,7 @@
         <v>2.78</v>
       </c>
     </row>
-    <row r="25" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C25">
         <f>C24-5</f>
         <v>-100</v>
@@ -9951,7 +9960,7 @@
         <v>2.89</v>
       </c>
     </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C26">
         <f t="shared" si="0"/>
         <v>-105</v>
@@ -9974,7 +9983,7 @@
         <v>3.01</v>
       </c>
     </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C27">
         <f t="shared" si="0"/>
         <v>-110</v>
@@ -9997,7 +10006,7 @@
         <v>3.14</v>
       </c>
     </row>
-    <row r="28" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C28">
         <f t="shared" si="0"/>
         <v>-115</v>
@@ -10020,7 +10029,7 @@
         <v>3.27</v>
       </c>
     </row>
-    <row r="29" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C29">
         <f>C28-5</f>
         <v>-120</v>
@@ -10043,7 +10052,7 @@
         <v>3.38</v>
       </c>
     </row>
-    <row r="30" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C30">
         <f t="shared" si="0"/>
         <v>-125</v>
@@ -10066,7 +10075,7 @@
         <v>3.48</v>
       </c>
     </row>
-    <row r="31" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C31">
         <f t="shared" si="0"/>
         <v>-130</v>
@@ -10089,7 +10098,7 @@
         <v>3.58</v>
       </c>
     </row>
-    <row r="32" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C32">
         <f t="shared" si="0"/>
         <v>-135</v>
@@ -10112,7 +10121,7 @@
         <v>3.66</v>
       </c>
     </row>
-    <row r="33" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C33">
         <f t="shared" si="0"/>
         <v>-140</v>
@@ -10135,7 +10144,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="34" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C34">
         <f t="shared" si="0"/>
         <v>-145</v>
@@ -10158,7 +10167,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="35" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C35">
         <f t="shared" si="0"/>
         <v>-150</v>
@@ -10181,7 +10190,7 @@
         <v>3.77</v>
       </c>
     </row>
-    <row r="36" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C36">
         <f t="shared" si="0"/>
         <v>-155</v>
@@ -10204,7 +10213,7 @@
         <v>3.76</v>
       </c>
     </row>
-    <row r="37" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C37">
         <f t="shared" si="0"/>
         <v>-160</v>
@@ -10227,7 +10236,7 @@
         <v>3.73</v>
       </c>
     </row>
-    <row r="38" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C38">
         <f t="shared" si="0"/>
         <v>-165</v>
@@ -10250,7 +10259,7 @@
         <v>3.68</v>
       </c>
     </row>
-    <row r="39" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C39">
         <f t="shared" si="0"/>
         <v>-170</v>

</xml_diff>